<commit_message>
deduplicating CSV records; corrected ClientCode from Young to Youth
</commit_message>
<xml_diff>
--- a/csv/unit_tests3.xlsx
+++ b/csv/unit_tests3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mie008443/work/compass/csv2turtle/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E2FDD3-D8EA-CE49-A3AF-ABF5AC879D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21627B6E-64A4-DE43-A6C3-5A03593CDF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20660" activeTab="1" xr2:uid="{A8202551-C63C-8A49-BB12-F636718BAEAD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20660" activeTab="4" xr2:uid="{A8202551-C63C-8A49-BB12-F636718BAEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stakeholders" sheetId="4" r:id="rId1"/>
@@ -362,30 +362,9 @@
     <t>Area0_Location</t>
   </si>
   <si>
-    <t>Shelter for young homeless women</t>
-  </si>
-  <si>
-    <t>Shelter for young women</t>
-  </si>
-  <si>
     <t>Shelter for homeless adults</t>
   </si>
   <si>
-    <t>Food for homeless young females</t>
-  </si>
-  <si>
-    <t>Food for young people</t>
-  </si>
-  <si>
-    <t>Food for young women</t>
-  </si>
-  <si>
-    <t>Education for homeless young females</t>
-  </si>
-  <si>
-    <t>education for young females</t>
-  </si>
-  <si>
     <t>Education for Homeless Adult males and females</t>
   </si>
   <si>
@@ -395,24 +374,12 @@
     <t>Health for Females</t>
   </si>
   <si>
-    <t>Health for young males</t>
-  </si>
-  <si>
     <t>LogicModel this service is a part of</t>
   </si>
   <si>
-    <t>Food for young males and adult females</t>
-  </si>
-  <si>
     <t>Food for homeless adults</t>
   </si>
   <si>
-    <t>Education for young females</t>
-  </si>
-  <si>
-    <t>Education for homeless young females, and homeles yong females</t>
-  </si>
-  <si>
     <t>P10-1</t>
   </si>
   <si>
@@ -1232,9 +1199,6 @@
     <t>cids:hasCode INST-Homeless, cids:hasCode INST-Adult, cids:hasCode INST-Male</t>
   </si>
   <si>
-    <t>cids:hasCode INST-Young, cids:hasCode INST-Male</t>
-  </si>
-  <si>
     <t>cids:hasCode INST-Adult, cids:hasCode INST-Male</t>
   </si>
   <si>
@@ -1251,6 +1215,42 @@
   </si>
   <si>
     <t>sh-Funder-in_Area0,sh-Funder-in_Area1</t>
+  </si>
+  <si>
+    <t>Shelter for Youth homeless women</t>
+  </si>
+  <si>
+    <t>Shelter for Youth women</t>
+  </si>
+  <si>
+    <t>Food for homeless Youth females</t>
+  </si>
+  <si>
+    <t>Food for Youth people</t>
+  </si>
+  <si>
+    <t>Food for Youth women</t>
+  </si>
+  <si>
+    <t>Education for homeless Youth females</t>
+  </si>
+  <si>
+    <t>education for Youth females</t>
+  </si>
+  <si>
+    <t>Health for Youth males</t>
+  </si>
+  <si>
+    <t>Food for Youth males and adult females</t>
+  </si>
+  <si>
+    <t>Education for homeless Youth females, and homeles yong females</t>
+  </si>
+  <si>
+    <t>Education for Youth females</t>
+  </si>
+  <si>
+    <t>cids:hasCode INST-Youth, cids:hasCode INST-Male</t>
   </si>
 </sst>
 </file>
@@ -1704,7 +1704,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B20"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1740,15 +1740,15 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="C3" t="s">
         <v>103</v>
@@ -1757,10 +1757,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="B4" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="C4" t="s">
         <v>103</v>
@@ -1769,10 +1769,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B5" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="C5" t="s">
         <v>103</v>
@@ -1781,10 +1781,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="C6" t="s">
         <v>103</v>
@@ -1793,10 +1793,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C7" t="s">
         <v>103</v>
@@ -1809,10 +1809,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B9" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="C9" t="s">
         <v>98</v>
@@ -1821,10 +1821,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="B10" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="C10" t="s">
         <v>98</v>
@@ -1833,10 +1833,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="B11" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="C11" t="s">
         <v>98</v>
@@ -1844,10 +1844,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="B12" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="C12" t="s">
         <v>98</v>
@@ -1855,10 +1855,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="B13" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C13" t="s">
         <v>98</v>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="B15" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="C15" t="s">
         <v>103</v>
@@ -1880,10 +1880,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="B16" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C16" t="s">
         <v>103</v>
@@ -1891,10 +1891,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="B17" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="C17" t="s">
         <v>98</v>
@@ -1902,10 +1902,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B18" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="C18" t="s">
         <v>98</v>
@@ -1913,10 +1913,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B19" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="C19" t="s">
         <v>103</v>
@@ -1924,10 +1924,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B20" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="C20" t="s">
         <v>98</v>
@@ -1943,7 +1943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4E49A9-2DA0-1E4E-8DC9-95F1075482B8}">
   <dimension ref="A2:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A41" sqref="A41:XFD42"/>
     </sheetView>
   </sheetViews>
@@ -1966,24 +1966,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="C3" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1992,7 +1992,7 @@
         <v>CL-Age</v>
       </c>
       <c r="C5" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2001,7 +2001,7 @@
         <v>CL-Age</v>
       </c>
       <c r="C6" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2010,7 +2010,7 @@
         <v>CL-Age</v>
       </c>
       <c r="C7" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2019,18 +2019,18 @@
         <v>CL-Age</v>
       </c>
       <c r="C8" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9" t="s">
         <v>268</v>
-      </c>
-      <c r="B9" t="s">
-        <v>273</v>
-      </c>
-      <c r="C9" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2039,7 +2039,7 @@
         <v>CL-Gender</v>
       </c>
       <c r="C10" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2048,7 +2048,7 @@
         <v>CL-Gender</v>
       </c>
       <c r="C11" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2057,18 +2057,18 @@
         <v>CL-Gender</v>
       </c>
       <c r="C12" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B13" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="C13" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2077,7 +2077,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C14" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2086,7 +2086,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C15" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2095,7 +2095,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C16" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2104,7 +2104,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C17" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2113,7 +2113,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C18" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2130,24 +2130,24 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B21" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C21" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2156,7 +2156,7 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C23" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2165,7 +2165,7 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C24" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2174,7 +2174,7 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C25" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2183,7 +2183,7 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C26" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2192,18 +2192,18 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C27" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2212,7 +2212,7 @@
         <v>CL-Education</v>
       </c>
       <c r="C29" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2221,7 +2221,7 @@
         <v>CL-Education</v>
       </c>
       <c r="C30" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2230,7 +2230,7 @@
         <v>CL-Education</v>
       </c>
       <c r="C31" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2239,18 +2239,18 @@
         <v>CL-Education</v>
       </c>
       <c r="C32" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2259,7 +2259,7 @@
         <v>CL-Food</v>
       </c>
       <c r="C34" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2268,7 +2268,7 @@
         <v>CL-Food</v>
       </c>
       <c r="C35" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2277,7 +2277,7 @@
         <v>CL-Food</v>
       </c>
       <c r="C36" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2286,18 +2286,18 @@
         <v>CL-Food</v>
       </c>
       <c r="C37" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2306,7 +2306,7 @@
         <v>CL-Health</v>
       </c>
       <c r="C39" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2315,7 +2315,7 @@
         <v>CL-Health</v>
       </c>
       <c r="C40" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2348,7 +2348,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>95</v>
@@ -2365,7 +2365,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
@@ -2379,10 +2379,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -2396,10 +2396,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="B4" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -2413,10 +2413,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="B5" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="C5">
         <v>40</v>
@@ -2430,10 +2430,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="B6" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="C6">
         <v>25</v>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B8" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -2464,10 +2464,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="B9" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -2481,10 +2481,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="B10" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="B11" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2515,10 +2515,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="B12" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2532,10 +2532,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="B14" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2549,10 +2549,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B15" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2566,10 +2566,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="B16" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2583,10 +2583,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B17" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2600,10 +2600,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B18" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2641,16 +2641,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -2669,19 +2669,19 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="E2" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="F2" t="s">
         <v>31</v>
@@ -2725,209 +2725,209 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="K3" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="L3" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="K4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="L4" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="K5" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="L5" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="K6" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="L6" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D7" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="K7" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="L7" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="K8" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="L8" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="K9" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="L9" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="K10" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="L10" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D12" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="K12" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="L12" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="M12" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2940,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C018D5EC-E981-8D4E-8560-6CCE31F45EF8}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G26"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2954,7 +2954,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>88</v>
@@ -3024,508 +3024,508 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>389</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="G3" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>390</v>
       </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F4" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="G4" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="G5" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>391</v>
       </c>
       <c r="E6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="G6" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>392</v>
       </c>
       <c r="E7" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="G7" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>393</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="F8" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="G8" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>394</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F9" t="s">
+        <v>347</v>
+      </c>
+      <c r="G9" t="s">
         <v>358</v>
-      </c>
-      <c r="G9" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>395</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="G10" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="G11" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C12" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F12" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="G12" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C13" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="G13" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D14" t="s">
-        <v>115</v>
+        <v>396</v>
       </c>
       <c r="E14" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="G14" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C15" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>397</v>
       </c>
       <c r="E15" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="G15" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>397</v>
       </c>
       <c r="E16" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="G16" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C18" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D18" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="E18" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F18" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="G18" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="E19" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F19" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="G19" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C20" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="D20" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="E20" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F20" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="G20" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C21" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D21" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="E21" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F21" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="G21" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D22" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="E22" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="F22" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="G22" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B23" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C23" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D23" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="E23" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="F23" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="G23" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B25" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C25" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="D25" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="E25" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F25" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="G25" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C26" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="D26" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="E26" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="F26" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="G26" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3582,464 +3582,464 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.CONCAT(A3, " Name")</f>
         <v>P10-1 Name</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>389</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F3" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ref="B4:B26" si="0">_xlfn.CONCAT(A4, " Name")</f>
         <v>P10-2 Name</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>390</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>P10-3 Name</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="E5" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>P11-1 Name</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>391</v>
       </c>
       <c r="D6" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>P11-2 Name</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>392</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="E7" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>P11-3 Name</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>393</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F8" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>P12-1n2 Name</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>398</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="E9" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F9" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>P12-1n2 Name</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>399</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>P12-3 Name</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E11" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>P13-1 Name</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F12" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>P13-2 Name</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="E13" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F13" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>P13-3 Name</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>396</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>P13-4 Name</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>397</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v>P13-4 Name</v>
       </c>
       <c r="C16" t="s">
-        <v>117</v>
+        <v>397</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E16" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>P20-a1 Name</v>
       </c>
       <c r="C18" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D18" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E18" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F18" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>P20-a2 Name</v>
       </c>
       <c r="C19" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D19" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="E19" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F19" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>P30-a3 Name</v>
       </c>
       <c r="C20" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D20" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="E20" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>P40-a4 Name</v>
       </c>
       <c r="C21" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D21" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E21" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F21" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>P40-a5 Name</v>
       </c>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D22" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E22" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F22" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>P50-a6na7 Name</v>
       </c>
       <c r="C23" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D23" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="E23" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F23" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v>P100-a100 Name</v>
       </c>
       <c r="C25" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D25" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="E25" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F25" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>P101-a101 Name</v>
       </c>
       <c r="C26" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="D26" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E26" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F26" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -4069,16 +4069,16 @@
   <sheetData>
     <row r="1" spans="1:15" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>52</v>
@@ -4091,7 +4091,7 @@
         <v>65</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>21</v>
@@ -4161,31 +4161,31 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>389</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="G3" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="H3" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="I3" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="J3" t="s">
         <v>49</v>
@@ -4193,31 +4193,31 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>390</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="H4" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="I4" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="J4" t="s">
         <v>49</v>
@@ -4225,31 +4225,31 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
         <v>126</v>
-      </c>
-      <c r="B5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" t="s">
-        <v>137</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="H5" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="I5" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="J5" t="s">
         <v>49</v>
@@ -4257,31 +4257,31 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>391</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="H6" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="I6" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="J6" t="s">
         <v>49</v>
@@ -4289,31 +4289,31 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>392</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="H7" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="I7" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="J7" t="s">
         <v>49</v>
@@ -4321,31 +4321,31 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" t="s">
+        <v>393</v>
+      </c>
+      <c r="D8" t="s">
         <v>129</v>
-      </c>
-      <c r="B8" t="s">
-        <v>245</v>
-      </c>
-      <c r="C8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" t="s">
-        <v>140</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="H8" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="I8" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="J8" t="s">
         <v>49</v>
@@ -4353,31 +4353,31 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" t="s">
+        <v>394</v>
+      </c>
+      <c r="D9" t="s">
         <v>130</v>
-      </c>
-      <c r="B9" t="s">
-        <v>246</v>
-      </c>
-      <c r="C9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" t="s">
-        <v>141</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="G9" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="H9" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="I9" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="J9" t="s">
         <v>49</v>
@@ -4385,31 +4385,31 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>395</v>
       </c>
       <c r="D10" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H10" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="I10" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="J10" t="s">
         <v>49</v>
@@ -4417,31 +4417,31 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="H11" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="I11" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="J11" t="s">
         <v>49</v>
@@ -4449,31 +4449,31 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H12" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="I12" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="J12" t="s">
         <v>49</v>
@@ -4481,31 +4481,31 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G13" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="H13" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="I13" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="J13" t="s">
         <v>49</v>
@@ -4513,31 +4513,31 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="H14" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="I14" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="J14" t="s">
         <v>49</v>
@@ -4545,31 +4545,31 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>396</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E15" t="s">
         <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="H15" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="I15" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="J15" t="s">
         <v>49</v>
@@ -4577,31 +4577,31 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C16" t="s">
-        <v>117</v>
+        <v>397</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="H16" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="I16" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="J16" t="s">
         <v>49</v>
@@ -4609,31 +4609,31 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>397</v>
       </c>
       <c r="D17" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H17" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="I17" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="J17" t="s">
         <v>49</v>
@@ -4641,204 +4641,204 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C19" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G19" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J19" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B20" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C20" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D20" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G20" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J20" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="C21" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="D21" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G21" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="J21" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B22" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C22" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D22" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="E22" t="s">
         <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G22" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="J22" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B23" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C23" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D23" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G23" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="J23" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B24" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="C24" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="D24" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E24" t="s">
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="G24" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="J24" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="B26" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="C26" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D26" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="E26" t="s">
         <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="J26" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B27" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C27" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D27" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="E27" t="s">
         <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="J27" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -4912,10 +4912,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -4924,10 +4924,10 @@
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4935,10 +4935,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -4947,10 +4947,10 @@
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4958,10 +4958,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D5">
         <v>120</v>
@@ -4970,10 +4970,10 @@
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -4981,10 +4981,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D6">
         <v>120</v>
@@ -4993,10 +4993,10 @@
         <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -5004,10 +5004,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D7">
         <v>120</v>
@@ -5016,10 +5016,10 @@
         <v>150</v>
       </c>
       <c r="F7" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -5027,10 +5027,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D8">
         <v>120</v>
@@ -5039,10 +5039,10 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -5050,10 +5050,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C9" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -5062,10 +5062,10 @@
         <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -5073,10 +5073,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D10">
         <v>40</v>
@@ -5085,10 +5085,10 @@
         <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -5096,10 +5096,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="D11">
         <v>55</v>
@@ -5108,10 +5108,10 @@
         <v>110</v>
       </c>
       <c r="F11" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -5119,10 +5119,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="D12">
         <v>110</v>
@@ -5131,10 +5131,10 @@
         <v>150</v>
       </c>
       <c r="F12" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -5142,10 +5142,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D13">
         <v>120</v>
@@ -5154,10 +5154,10 @@
         <v>150</v>
       </c>
       <c r="F13" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G13" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -5165,10 +5165,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D14">
         <v>20</v>
@@ -5177,10 +5177,10 @@
         <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -5188,10 +5188,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C15" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D15">
         <v>120</v>
@@ -5200,10 +5200,10 @@
         <v>150</v>
       </c>
       <c r="F15" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -5211,10 +5211,10 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C16" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D16">
         <v>50</v>
@@ -5223,10 +5223,10 @@
         <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -5234,10 +5234,10 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C18" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D18">
         <v>200</v>
@@ -5246,10 +5246,10 @@
         <v>300</v>
       </c>
       <c r="F18" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G18" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -5257,10 +5257,10 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C19" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D19">
         <v>200</v>
@@ -5269,10 +5269,10 @@
         <v>300</v>
       </c>
       <c r="F19" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="G19" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -5280,10 +5280,10 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C20" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D20">
         <v>200</v>
@@ -5292,21 +5292,21 @@
         <v>300</v>
       </c>
       <c r="F20" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="G20" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B21" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C21" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D21">
         <v>100</v>
@@ -5315,21 +5315,21 @@
         <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G21" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B22" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C22" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D22">
         <v>100</v>
@@ -5338,21 +5338,21 @@
         <v>105</v>
       </c>
       <c r="F22" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="G22" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B23" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C23" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D23">
         <v>100</v>
@@ -5361,10 +5361,10 @@
         <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="G23" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected service hasCode in excel.
</commit_message>
<xml_diff>
--- a/csv/unit_tests3.xlsx
+++ b/csv/unit_tests3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mie008443/work/compass/csv2turtle/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21627B6E-64A4-DE43-A6C3-5A03593CDF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8D32C9-77F5-414C-A7D6-471E8E398B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20660" activeTab="4" xr2:uid="{A8202551-C63C-8A49-BB12-F636718BAEAD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20660" activeTab="1" xr2:uid="{A8202551-C63C-8A49-BB12-F636718BAEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stakeholders" sheetId="4" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>CL-Education</t>
   </si>
   <si>
-    <t>CL-Funding</t>
-  </si>
-  <si>
     <t>Funding label</t>
   </si>
   <si>
@@ -1251,6 +1248,9 @@
   </si>
   <si>
     <t>cids:hasCode INST-Youth, cids:hasCode INST-Male</t>
+  </si>
+  <si>
+    <t>sh-Adult-Female-Homeless-in_Area0, sh-Adult-Male-Homeless-in_Area1</t>
   </si>
 </sst>
 </file>
@@ -1715,13 +1715,13 @@
   <sheetData>
     <row r="1" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -1731,75 +1731,75 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
       <c r="D2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1809,59 +1809,59 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1869,68 +1869,68 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1943,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4E49A9-2DA0-1E4E-8DC9-95F1075482B8}">
   <dimension ref="A2:C43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD42"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1955,35 +1955,35 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1992,7 +1992,7 @@
         <v>CL-Age</v>
       </c>
       <c r="C5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2001,7 +2001,7 @@
         <v>CL-Age</v>
       </c>
       <c r="C6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2010,7 +2010,7 @@
         <v>CL-Age</v>
       </c>
       <c r="C7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2019,18 +2019,18 @@
         <v>CL-Age</v>
       </c>
       <c r="C8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2039,7 +2039,7 @@
         <v>CL-Gender</v>
       </c>
       <c r="C10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2048,7 +2048,7 @@
         <v>CL-Gender</v>
       </c>
       <c r="C11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2057,18 +2057,18 @@
         <v>CL-Gender</v>
       </c>
       <c r="C12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2077,7 +2077,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2086,7 +2086,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2095,7 +2095,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2104,7 +2104,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2113,7 +2113,7 @@
         <v>CL-Housing_State</v>
       </c>
       <c r="C18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2130,24 +2130,24 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2156,7 +2156,7 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2165,7 +2165,7 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2174,7 +2174,7 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2183,7 +2183,7 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2192,18 +2192,18 @@
         <v>CL-Shelter</v>
       </c>
       <c r="C27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2212,7 +2212,7 @@
         <v>CL-Education</v>
       </c>
       <c r="C29" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2221,7 +2221,7 @@
         <v>CL-Education</v>
       </c>
       <c r="C30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2230,7 +2230,7 @@
         <v>CL-Education</v>
       </c>
       <c r="C31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2239,18 +2239,18 @@
         <v>CL-Education</v>
       </c>
       <c r="C32" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2259,7 +2259,7 @@
         <v>CL-Food</v>
       </c>
       <c r="C34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2268,7 +2268,7 @@
         <v>CL-Food</v>
       </c>
       <c r="C35" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2277,7 +2277,7 @@
         <v>CL-Food</v>
       </c>
       <c r="C36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2286,18 +2286,18 @@
         <v>CL-Food</v>
       </c>
       <c r="C37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2306,7 +2306,7 @@
         <v>CL-Health</v>
       </c>
       <c r="C39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2315,7 +2315,7 @@
         <v>CL-Health</v>
       </c>
       <c r="C40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2345,19 +2345,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2365,254 +2365,254 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
         <v>96</v>
-      </c>
-      <c r="E2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C3">
         <v>50</v>
       </c>
       <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
         <v>102</v>
-      </c>
-      <c r="E3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C4">
         <v>30</v>
       </c>
       <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
         <v>102</v>
-      </c>
-      <c r="E4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C5">
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C6">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
         <v>102</v>
-      </c>
-      <c r="E8" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
         <v>102</v>
-      </c>
-      <c r="E9" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" t="s">
         <v>102</v>
-      </c>
-      <c r="E10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" t="s">
         <v>102</v>
-      </c>
-      <c r="E11" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" t="s">
         <v>102</v>
-      </c>
-      <c r="E12" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2641,16 +2641,16 @@
   <sheetData>
     <row r="1" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -2669,265 +2669,265 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E2" t="s">
-        <v>253</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="L2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>37</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>40</v>
-      </c>
-      <c r="R2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" t="s">
         <v>186</v>
       </c>
-      <c r="D12" t="s">
+      <c r="J12" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="K12" t="s">
         <v>187</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="K12" t="s">
-        <v>188</v>
-      </c>
       <c r="L12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2940,7 +2940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C018D5EC-E981-8D4E-8560-6CCE31F45EF8}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2954,578 +2954,578 @@
   <sheetData>
     <row r="1" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>90</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="J1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>70</v>
       </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" t="s">
         <v>82</v>
-      </c>
-      <c r="K2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F21" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F23" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" t="s">
+        <v>227</v>
+      </c>
+      <c r="D25" t="s">
         <v>194</v>
       </c>
-      <c r="B25" t="s">
-        <v>188</v>
-      </c>
-      <c r="C25" t="s">
-        <v>228</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>195</v>
       </c>
-      <c r="E25" t="s">
-        <v>196</v>
-      </c>
       <c r="F25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" t="s">
         <v>194</v>
       </c>
-      <c r="B26" t="s">
-        <v>188</v>
-      </c>
-      <c r="C26" t="s">
-        <v>228</v>
-      </c>
-      <c r="D26" t="s">
-        <v>195</v>
-      </c>
       <c r="E26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3555,7 +3555,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3565,481 +3565,481 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.CONCAT(A3, " Name")</f>
         <v>P10-1 Name</v>
       </c>
       <c r="C3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ref="B4:B26" si="0">_xlfn.CONCAT(A4, " Name")</f>
         <v>P10-2 Name</v>
       </c>
       <c r="C4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
         <v>P10-3 Name</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>P11-1 Name</v>
       </c>
       <c r="C6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>P11-2 Name</v>
       </c>
       <c r="C7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>P11-3 Name</v>
       </c>
       <c r="C8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>P12-1n2 Name</v>
       </c>
       <c r="C9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>P12-1n2 Name</v>
       </c>
       <c r="C10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>P12-3 Name</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>P13-1 Name</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E12" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>P13-2 Name</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>P13-3 Name</v>
       </c>
       <c r="C14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>P13-4 Name</v>
       </c>
       <c r="C15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v>P13-4 Name</v>
       </c>
       <c r="C16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>P20-a1 Name</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>P20-a2 Name</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F19" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>P30-a3 Name</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>P40-a4 Name</v>
       </c>
       <c r="C21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>P40-a5 Name</v>
       </c>
       <c r="C22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>P50-a6na7 Name</v>
       </c>
       <c r="C23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v>P100-a100 Name</v>
       </c>
       <c r="C25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>P101-a101 Name</v>
       </c>
       <c r="C26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E26" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F26" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -4052,8 +4052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A168A40-4F98-2D4B-9B19-5D3AF53C327F}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I27"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4069,47 +4069,47 @@
   <sheetData>
     <row r="1" spans="1:15" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -4117,728 +4117,728 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
         <v>56</v>
       </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N2" t="s">
-        <v>57</v>
-      </c>
       <c r="O2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>275</v>
       </c>
       <c r="F3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>275</v>
       </c>
       <c r="F4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>279</v>
       </c>
       <c r="F5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>369</v>
+        <v>400</v>
       </c>
       <c r="H5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>279</v>
       </c>
       <c r="F6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>279</v>
       </c>
       <c r="F7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>279</v>
       </c>
       <c r="F8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>276</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>276</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>276</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>276</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>282</v>
       </c>
       <c r="F13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>282</v>
       </c>
       <c r="F14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>282</v>
       </c>
       <c r="F15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>279</v>
       </c>
       <c r="F16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>279</v>
       </c>
       <c r="F17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="F19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="F20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="F21" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="F22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="F23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="F24" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="G26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>342</v>
       </c>
       <c r="G27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -4863,25 +4863,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -4889,22 +4889,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -4912,10 +4912,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -4924,10 +4924,10 @@
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4935,10 +4935,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -4947,10 +4947,10 @@
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4958,10 +4958,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D5">
         <v>120</v>
@@ -4970,10 +4970,10 @@
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -4981,10 +4981,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D6">
         <v>120</v>
@@ -4993,10 +4993,10 @@
         <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -5004,10 +5004,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7">
         <v>120</v>
@@ -5016,10 +5016,10 @@
         <v>150</v>
       </c>
       <c r="F7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -5027,10 +5027,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D8">
         <v>120</v>
@@ -5039,10 +5039,10 @@
         <v>150</v>
       </c>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -5050,10 +5050,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -5062,10 +5062,10 @@
         <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -5073,10 +5073,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D10">
         <v>40</v>
@@ -5085,10 +5085,10 @@
         <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -5096,10 +5096,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D11">
         <v>55</v>
@@ -5108,10 +5108,10 @@
         <v>110</v>
       </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -5119,10 +5119,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D12">
         <v>110</v>
@@ -5131,10 +5131,10 @@
         <v>150</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -5142,10 +5142,10 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D13">
         <v>120</v>
@@ -5154,10 +5154,10 @@
         <v>150</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -5165,10 +5165,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D14">
         <v>20</v>
@@ -5177,10 +5177,10 @@
         <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -5188,10 +5188,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D15">
         <v>120</v>
@@ -5200,10 +5200,10 @@
         <v>150</v>
       </c>
       <c r="F15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -5211,10 +5211,10 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D16">
         <v>50</v>
@@ -5223,21 +5223,21 @@
         <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D18">
         <v>200</v>
@@ -5246,21 +5246,21 @@
         <v>300</v>
       </c>
       <c r="F18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19">
         <v>200</v>
@@ -5269,21 +5269,21 @@
         <v>300</v>
       </c>
       <c r="F19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D20">
         <v>200</v>
@@ -5292,21 +5292,21 @@
         <v>300</v>
       </c>
       <c r="F20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D21">
         <v>100</v>
@@ -5315,21 +5315,21 @@
         <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D22">
         <v>100</v>
@@ -5338,21 +5338,21 @@
         <v>105</v>
       </c>
       <c r="F22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23">
         <v>100</v>
@@ -5361,10 +5361,10 @@
         <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ServiceFailureEvent; updated Excel file with ServiceFailreEvents and made Funding names unique
</commit_message>
<xml_diff>
--- a/csv/unit_tests3.xlsx
+++ b/csv/unit_tests3.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="523">
   <si>
     <t>Stakeholder instances</t>
   </si>
@@ -30,12 +30,12 @@
     <t>Stakeholder</t>
   </si>
   <si>
+    <t>sh-Adult-Female-Homeless-in_Area0</t>
+  </si>
+  <si>
     <t>sh-Homeless-Female-Youth-in_Area0</t>
   </si>
   <si>
-    <t>sh-Adult-Female-Homeless-in_Area0</t>
-  </si>
-  <si>
     <t>sh-Funder-in_Area0</t>
   </si>
   <si>
@@ -45,12 +45,12 @@
     <t>sh-Adult-Male-Homeless-in_Area0</t>
   </si>
   <si>
+    <t>sh-Adult-Female-Homeless-in_Area1</t>
+  </si>
+  <si>
     <t>sh-Homeless-Female-Youth-in_Area1</t>
   </si>
   <si>
-    <t>sh-Adult-Female-Homeless-in_Area1</t>
-  </si>
-  <si>
     <t>sh-Homeless-in_Area1</t>
   </si>
   <si>
@@ -81,12 +81,12 @@
     <t>sh-Female-Youth-in_Area0</t>
   </si>
   <si>
+    <t>sh-Adult-Female-in_Area1</t>
+  </si>
+  <si>
     <t>sh-Female-Youth-in_Area1</t>
   </si>
   <si>
-    <t>sh-Adult-Female-in_Area1</t>
-  </si>
-  <si>
     <t>sh-Adult-Homeless-Male-in_Area1</t>
   </si>
   <si>
@@ -168,12 +168,12 @@
     <t>hasCode</t>
   </si>
   <si>
+    <t>INST-Adult,INST-Female,INST-Homeless</t>
+  </si>
+  <si>
     <t>INST-Female,INST-Homeless,INST-Youth</t>
   </si>
   <si>
-    <t>INST-Adult,INST-Female,INST-Homeless</t>
-  </si>
-  <si>
     <t>INST-Funder</t>
   </si>
   <si>
@@ -1479,12 +1479,6 @@
     <t>hasFocus</t>
   </si>
   <si>
-    <t>cids:hasCode INST-Female,cids:hasCode INST-Youth</t>
-  </si>
-  <si>
-    <t>cids:hasCode INST-Adult, cids:hasCode INST-Male</t>
-  </si>
-  <si>
     <t>Characteristics of the community</t>
   </si>
   <si>
@@ -1527,31 +1521,31 @@
     <t>Funding</t>
   </si>
   <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>a7</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>a4</t>
-  </si>
-  <si>
-    <t>a5</t>
-  </si>
-  <si>
-    <t>a6</t>
-  </si>
-  <si>
-    <t>a100</t>
-  </si>
-  <si>
-    <t>a101</t>
+    <t>a1-for-P20-a1</t>
+  </si>
+  <si>
+    <t>a2-for-P20-a2</t>
+  </si>
+  <si>
+    <t>a7-for-P50-a6na7</t>
+  </si>
+  <si>
+    <t>a3-for-P30-a3</t>
+  </si>
+  <si>
+    <t>a4-for-P40-a4</t>
+  </si>
+  <si>
+    <t>a5-for-P40-a5</t>
+  </si>
+  <si>
+    <t>a6-for-P50-a6na7</t>
+  </si>
+  <si>
+    <t>a100-for-P100-a100</t>
+  </si>
+  <si>
+    <t>a101-for-P101-a101</t>
   </si>
   <si>
     <t>links to organization providing the funds.</t>
@@ -2153,7 +2147,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
         <v>82</v>
@@ -2197,7 +2191,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
         <v>83</v>
@@ -2208,7 +2202,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
         <v>83</v>
@@ -4210,7 +4204,7 @@
         <v>331</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
         <v>361</v>
@@ -4279,7 +4273,7 @@
         <v>334</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
         <v>362</v>
@@ -4302,7 +4296,7 @@
         <v>335</v>
       </c>
       <c r="F7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
         <v>364</v>
@@ -4371,7 +4365,7 @@
         <v>337</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
         <v>365</v>
@@ -4394,7 +4388,7 @@
         <v>338</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
         <v>366</v>
@@ -4463,7 +4457,7 @@
         <v>341</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
         <v>364</v>
@@ -4486,7 +4480,7 @@
         <v>342</v>
       </c>
       <c r="F15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G15" t="s">
         <v>364</v>
@@ -4509,7 +4503,7 @@
         <v>342</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16" t="s">
         <v>369</v>
@@ -4706,7 +4700,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4882,7 +4876,7 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4902,7 +4896,7 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5007,36 +5001,36 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B16" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C16" t="s">
-        <v>323</v>
+        <v>402</v>
       </c>
       <c r="D16" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E16" t="s">
-        <v>434</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>437</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B17" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C17" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D17" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E17" t="s">
         <v>4</v>
@@ -5047,56 +5041,56 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B18" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C18" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D18" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B19" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C19" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D19" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B20" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C20" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D20" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -5107,81 +5101,61 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B21" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C21" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D21" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>434</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>438</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B22" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C22" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D22" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E22" t="s">
         <v>434</v>
       </c>
       <c r="F22" t="s">
-        <v>438</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B23" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C23" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D23" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E23" t="s">
         <v>434</v>
       </c>
       <c r="F23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>350</v>
-      </c>
-      <c r="B24" t="s">
-        <v>398</v>
-      </c>
-      <c r="C24" t="s">
-        <v>409</v>
-      </c>
-      <c r="D24" t="s">
-        <v>432</v>
-      </c>
-      <c r="E24" t="s">
-        <v>434</v>
-      </c>
-      <c r="F24" t="s">
         <v>359</v>
       </c>
     </row>
@@ -5231,22 +5205,22 @@
         <v>483</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -5281,13 +5255,13 @@
         <v>484</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>495</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>371</v>
@@ -5331,7 +5305,7 @@
         <v>471</v>
       </c>
       <c r="K3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -5366,7 +5340,7 @@
         <v>362</v>
       </c>
       <c r="K4" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -5401,7 +5375,7 @@
         <v>472</v>
       </c>
       <c r="K5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -5436,7 +5410,7 @@
         <v>471</v>
       </c>
       <c r="K6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -5471,7 +5445,7 @@
         <v>362</v>
       </c>
       <c r="K7" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -5506,7 +5480,7 @@
         <v>473</v>
       </c>
       <c r="K8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -5529,7 +5503,7 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s">
         <v>473</v>
@@ -5538,10 +5512,10 @@
         <v>482</v>
       </c>
       <c r="J9" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="K9" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -5564,7 +5538,7 @@
         <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
         <v>474</v>
@@ -5576,7 +5550,7 @@
         <v>474</v>
       </c>
       <c r="K10" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -5599,7 +5573,7 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" t="s">
         <v>475</v>
@@ -5611,7 +5585,7 @@
         <v>475</v>
       </c>
       <c r="K11" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -5646,7 +5620,7 @@
         <v>476</v>
       </c>
       <c r="K12" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -5681,7 +5655,7 @@
         <v>367</v>
       </c>
       <c r="K13" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -5716,7 +5690,7 @@
         <v>368</v>
       </c>
       <c r="K14" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -5751,7 +5725,7 @@
         <v>477</v>
       </c>
       <c r="K15" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -5786,7 +5760,7 @@
         <v>477</v>
       </c>
       <c r="K16" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -5818,10 +5792,10 @@
         <v>481</v>
       </c>
       <c r="J17" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="K17" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -5847,7 +5821,7 @@
         <v>11</v>
       </c>
       <c r="K18" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -5873,7 +5847,7 @@
         <v>11</v>
       </c>
       <c r="K19" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -5899,7 +5873,7 @@
         <v>12</v>
       </c>
       <c r="K20" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -5925,7 +5899,7 @@
         <v>13</v>
       </c>
       <c r="K21" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -5951,7 +5925,7 @@
         <v>13</v>
       </c>
       <c r="K22" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -5977,7 +5951,7 @@
         <v>12</v>
       </c>
       <c r="K23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -6003,7 +5977,7 @@
         <v>14</v>
       </c>
       <c r="K24" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -6026,7 +6000,7 @@
         <v>4</v>
       </c>
       <c r="K25" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -6049,7 +6023,7 @@
         <v>4</v>
       </c>
       <c r="K26" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -6072,7 +6046,7 @@
         <v>5</v>
       </c>
       <c r="K27" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -6093,53 +6067,53 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B3" t="s">
         <v>229</v>
@@ -6157,12 +6131,12 @@
         <v>331</v>
       </c>
       <c r="G3" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B4" t="s">
         <v>229</v>
@@ -6180,12 +6154,12 @@
         <v>332</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B5" t="s">
         <v>229</v>
@@ -6203,12 +6177,12 @@
         <v>333</v>
       </c>
       <c r="G5" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B6" t="s">
         <v>229</v>
@@ -6226,12 +6200,12 @@
         <v>334</v>
       </c>
       <c r="G6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B7" t="s">
         <v>229</v>
@@ -6249,12 +6223,12 @@
         <v>335</v>
       </c>
       <c r="G7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B8" t="s">
         <v>232</v>
@@ -6277,7 +6251,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B9" t="s">
         <v>230</v>
@@ -6300,7 +6274,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B10" t="s">
         <v>230</v>
@@ -6323,7 +6297,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B11" t="s">
         <v>231</v>
@@ -6346,7 +6320,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B12" t="s">
         <v>231</v>
@@ -6364,12 +6338,12 @@
         <v>338</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B13" t="s">
         <v>232</v>
@@ -6392,7 +6366,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B14" t="s">
         <v>232</v>
@@ -6415,7 +6389,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B15" t="s">
         <v>232</v>
@@ -6433,12 +6407,12 @@
         <v>341</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B16" t="s">
         <v>232</v>
@@ -6456,12 +6430,12 @@
         <v>342</v>
       </c>
       <c r="G16" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B18" t="s">
         <v>233</v>
@@ -6484,7 +6458,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B19" t="s">
         <v>233</v>
@@ -6507,7 +6481,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B20" t="s">
         <v>233</v>
@@ -6530,7 +6504,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B21" t="s">
         <v>233</v>
@@ -6553,7 +6527,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B22" t="s">
         <v>233</v>
@@ -6576,7 +6550,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B23" t="s">
         <v>233</v>

</xml_diff>

<commit_message>
corrected Organization.hasOutcome, removed Organization.hasIdentifier placeholder
</commit_message>
<xml_diff>
--- a/csv/unit_tests3.xlsx
+++ b/csv/unit_tests3.xlsx
@@ -30,12 +30,12 @@
     <t>Stakeholder</t>
   </si>
   <si>
+    <t>sh-Homeless-Female-Youth-in_Area0</t>
+  </si>
+  <si>
     <t>sh-Adult-Female-Homeless-in_Area0</t>
   </si>
   <si>
-    <t>sh-Homeless-Female-Youth-in_Area0</t>
-  </si>
-  <si>
     <t>sh-Funder-in_Area0</t>
   </si>
   <si>
@@ -45,12 +45,12 @@
     <t>sh-Adult-Male-Homeless-in_Area0</t>
   </si>
   <si>
+    <t>sh-Homeless-Female-Youth-in_Area1</t>
+  </si>
+  <si>
     <t>sh-Adult-Female-Homeless-in_Area1</t>
   </si>
   <si>
-    <t>sh-Homeless-Female-Youth-in_Area1</t>
-  </si>
-  <si>
     <t>sh-Homeless-in_Area1</t>
   </si>
   <si>
@@ -168,10 +168,10 @@
     <t>hasCode</t>
   </si>
   <si>
+    <t>INST-Female,INST-Homeless,INST-Youth</t>
+  </si>
+  <si>
     <t>INST-Adult,INST-Female,INST-Homeless</t>
-  </si>
-  <si>
-    <t>INST-Female,INST-Homeless,INST-Youth</t>
   </si>
   <si>
     <t>INST-Funder</t>
@@ -2147,7 +2147,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
         <v>82</v>
@@ -4204,7 +4204,7 @@
         <v>331</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
         <v>361</v>
@@ -4273,7 +4273,7 @@
         <v>334</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" t="s">
         <v>362</v>
@@ -4296,7 +4296,7 @@
         <v>335</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" t="s">
         <v>364</v>
@@ -4365,7 +4365,7 @@
         <v>337</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" t="s">
         <v>365</v>
@@ -4388,7 +4388,7 @@
         <v>338</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
         <v>366</v>
@@ -4457,7 +4457,7 @@
         <v>341</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" t="s">
         <v>364</v>
@@ -4480,7 +4480,7 @@
         <v>342</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
         <v>364</v>
@@ -4503,7 +4503,7 @@
         <v>342</v>
       </c>
       <c r="F16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G16" t="s">
         <v>369</v>
@@ -5573,7 +5573,7 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H11" t="s">
         <v>475</v>
@@ -6154,7 +6154,7 @@
         <v>332</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6200,7 +6200,7 @@
         <v>334</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6223,7 +6223,7 @@
         <v>335</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6338,7 +6338,7 @@
         <v>338</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6407,7 +6407,7 @@
         <v>341</v>
       </c>
       <c r="G15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7">

</xml_diff>